<commit_message>
$BMBL metrics for historical AR
</commit_message>
<xml_diff>
--- a/Overview - Dating Apps.xlsx
+++ b/Overview - Dating Apps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572903DF-2775-4913-999F-5D496B6BFA67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F797B1-27F2-426A-B401-2F23283E34CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2640" yWindow="2070" windowWidth="26610" windowHeight="12885" xr2:uid="{8DD4D602-3D6B-425D-835C-57218E4C1C6C}"/>
+    <workbookView xWindow="2205" yWindow="960" windowWidth="26610" windowHeight="12885" xr2:uid="{8DD4D602-3D6B-425D-835C-57218E4C1C6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -649,24 +649,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -677,6 +659,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -708,66 +708,62 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>11.03</v>
+            <v>10.68</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>1612.5039999999999</v>
+            <v>134.936824</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>17785.919119999999</v>
+            <v>1441.12528032</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-205.32000000000016</v>
+            <v>-265.28400000000005</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>17991.239119999998</v>
+            <v>1706.4092803200001</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Santa Monica, CA</v>
+            <v>Austin, TX</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>2010</v>
+            <v>2006</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>42795</v>
+            <v>44228</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>414</v>
+            <v>3.7206999999999999</v>
           </cell>
         </row>
         <row r="28">
           <cell r="C28">
-            <v>3.29</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="C29">
-            <v>5289</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="C31" t="str">
-            <v>FY23</v>
+            <v>23.03</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="44">
+          <cell r="W44">
+            <v>1200</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -784,62 +780,66 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>10.68</v>
+            <v>11.03</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>134.936824</v>
+            <v>1612.5039999999999</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>1441.12528032</v>
+            <v>17785.919119999999</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-265.28400000000005</v>
+            <v>-205.32000000000016</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>1706.4092803200001</v>
+            <v>17991.239119999998</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Austin, TX</v>
+            <v>Santa Monica, CA</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>2006</v>
+            <v>2010</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>44228</v>
+            <v>42795</v>
           </cell>
         </row>
         <row r="27">
           <cell r="C27">
-            <v>3.7206999999999999</v>
+            <v>414</v>
           </cell>
         </row>
         <row r="28">
           <cell r="C28">
-            <v>23.03</v>
+            <v>3.29</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="C29">
+            <v>5289</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="C31" t="str">
+            <v>FY23</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="44">
-          <cell r="W44">
-            <v>1200</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1148,7 +1148,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E12:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1173,16 +1173,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26">
-      <c r="Q1" s="53" t="s">
+      <c r="Q1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="53"/>
+      <c r="T1" s="47"/>
     </row>
     <row r="2" spans="2:26" s="2" customFormat="1">
       <c r="B2" s="2" t="s">
@@ -1327,52 +1327,52 @@
       <c r="E5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="51">
-        <f>[2]Main!$C$6</f>
+      <c r="F5" s="45">
+        <f>[1]Main!$C$6</f>
         <v>10.68</v>
       </c>
       <c r="G5" s="10">
-        <f>[2]Main!$C$7</f>
+        <f>[1]Main!$C$7</f>
         <v>134.936824</v>
       </c>
       <c r="H5" s="13">
-        <f>[2]Main!$C$8</f>
+        <f>[1]Main!$C$8</f>
         <v>1441.12528032</v>
       </c>
       <c r="I5" s="10">
-        <f>[2]Main!$C$11</f>
+        <f>[1]Main!$C$11</f>
         <v>-265.28400000000005</v>
       </c>
       <c r="J5" s="10">
-        <f>[2]Main!$C$12</f>
+        <f>[1]Main!$C$12</f>
         <v>1706.4092803200001</v>
       </c>
       <c r="K5" s="11" t="s">
         <v>72</v>
       </c>
       <c r="M5" s="4"/>
-      <c r="Q5" s="52">
-        <f>[2]Main!$C$27</f>
+      <c r="Q5" s="46">
+        <f>[1]Main!$C$27</f>
         <v>3.7206999999999999</v>
       </c>
-      <c r="S5" s="54">
-        <f>[2]Main!$C$28</f>
+      <c r="S5" s="48">
+        <f>[1]Main!$C$28</f>
         <v>23.03</v>
       </c>
       <c r="T5" s="44">
-        <f>'[2]Financial Model'!$W$44</f>
+        <f>'[1]Financial Model'!$W$44</f>
         <v>1200</v>
       </c>
       <c r="V5" s="4" t="str">
-        <f>+[2]Main!$C$23</f>
+        <f>+[1]Main!$C$23</f>
         <v>Austin, TX</v>
       </c>
       <c r="W5" s="4">
-        <f>+[2]Main!$C$24</f>
+        <f>+[1]Main!$C$24</f>
         <v>2006</v>
       </c>
       <c r="X5" s="14">
-        <f>+[2]Main!$C$25</f>
+        <f>+[1]Main!$C$25</f>
         <v>44228</v>
       </c>
       <c r="Y5" s="14"/>
@@ -1457,52 +1457,52 @@
         <v>31</v>
       </c>
       <c r="F9" s="41">
-        <f>+[1]Main!$C$6</f>
+        <f>+[2]Main!$C$6</f>
         <v>11.03</v>
       </c>
       <c r="G9" s="10">
-        <f>+[1]Main!$C$7</f>
+        <f>+[2]Main!$C$7</f>
         <v>1612.5039999999999</v>
       </c>
       <c r="H9" s="13">
-        <f>+[1]Main!$C$8</f>
+        <f>+[2]Main!$C$8</f>
         <v>17785.919119999999</v>
       </c>
       <c r="I9" s="10">
-        <f>+[1]Main!$C$11</f>
+        <f>+[2]Main!$C$11</f>
         <v>-205.32000000000016</v>
       </c>
       <c r="J9" s="10">
-        <f>+[1]Main!$C$12</f>
+        <f>+[2]Main!$C$12</f>
         <v>17991.239119999998</v>
       </c>
       <c r="K9" s="11" t="str">
-        <f>+[1]Main!$C$31</f>
+        <f>+[2]Main!$C$31</f>
         <v>FY23</v>
       </c>
       <c r="M9" s="4"/>
       <c r="R9" s="4">
-        <f>[1]Main!$C$27</f>
+        <f>[2]Main!$C$27</f>
         <v>414</v>
       </c>
       <c r="S9" s="4">
-        <f>[1]Main!$C$28</f>
+        <f>[2]Main!$C$28</f>
         <v>3.29</v>
       </c>
       <c r="T9" s="44">
-        <f>[1]Main!$C$29</f>
+        <f>[2]Main!$C$29</f>
         <v>5289</v>
       </c>
       <c r="V9" s="4" t="str">
-        <f>+[1]Main!$C$23</f>
+        <f>+[2]Main!$C$23</f>
         <v>Santa Monica, CA</v>
       </c>
       <c r="W9" s="4">
-        <f>+[1]Main!$C$24</f>
+        <f>+[2]Main!$C$24</f>
         <v>2010</v>
       </c>
       <c r="X9" s="14">
-        <f>+[1]Main!$C$25</f>
+        <f>+[2]Main!$C$25</f>
         <v>42795</v>
       </c>
       <c r="Y9" s="14"/>
@@ -1593,14 +1593,14 @@
       <c r="B3" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="R3" s="45" t="s">
+      <c r="R3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="46"/>
-      <c r="T3" s="47" t="s">
+      <c r="S3" s="50"/>
+      <c r="T3" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="46"/>
+      <c r="U3" s="50"/>
     </row>
     <row r="4" spans="2:21">
       <c r="B4" s="24" t="s">
@@ -1682,12 +1682,12 @@
       </c>
     </row>
     <row r="14" spans="2:21">
-      <c r="R14" s="48" t="s">
+      <c r="R14" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="S14" s="49"/>
-      <c r="T14" s="49"/>
-      <c r="U14" s="50"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="54"/>
     </row>
     <row r="15" spans="2:21">
       <c r="B15" s="26" t="s">

</xml_diff>